<commit_message>
meer uitgewerkte game analytics + game analytics code is uitgecomment
</commit_message>
<xml_diff>
--- a/Game Analytics/Game Analytics.xlsx
+++ b/Game Analytics/Game Analytics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>pick ups</t>
   </si>
@@ -61,13 +61,19 @@
   <si>
     <t>Level 4</t>
   </si>
+  <si>
+    <t>deaths</t>
+  </si>
+  <si>
+    <t>avg. Deaths</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -98,15 +104,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -442,11 +477,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="563786816"/>
-        <c:axId val="563790080"/>
+        <c:axId val="-273112640"/>
+        <c:axId val="-273112096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="563786816"/>
+        <c:axId val="-273112640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -486,7 +521,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="563790080"/>
+        <c:crossAx val="-273112096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -494,7 +529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="563790080"/>
+        <c:axId val="-273112096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +577,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="563786816"/>
+        <c:crossAx val="-273112640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -620,7 +655,355 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>Average Player Deaths</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Blad1!$B$3:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Level 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Level 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Level 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Level 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$L$3:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.3888888888888888</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17647058823529413</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.25E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="-273109376"/>
+        <c:axId val="-273107200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-273109376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-273107200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-273107200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-273109376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1129,6 +1512,475 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1156,6 +2008,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Grafiek 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1427,10 +2309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I6"/>
+  <dimension ref="B2:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,9 +2320,10 @@
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -1465,8 +2348,14 @@
       <c r="I2" t="s">
         <v>7</v>
       </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -1494,8 +2383,15 @@
         <f>F3/C3</f>
         <v>2.3333333333333335</v>
       </c>
+      <c r="K3">
+        <v>43</v>
+      </c>
+      <c r="L3" s="2">
+        <f>K3/C3</f>
+        <v>2.3888888888888888</v>
+      </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -1523,8 +2419,15 @@
         <f>F4/C4</f>
         <v>10.666666666666666</v>
       </c>
+      <c r="K4">
+        <v>14</v>
+      </c>
+      <c r="L4" s="2">
+        <f>K4/C4</f>
+        <v>0.77777777777777779</v>
+      </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -1552,8 +2455,15 @@
         <f>F5/C5</f>
         <v>6.2352941176470589</v>
       </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2">
+        <f>K5/C5</f>
+        <v>0.17647058823529413</v>
+      </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -1580,6 +2490,13 @@
       <c r="I6" s="1">
         <f>F6/C6</f>
         <v>5</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <f>K6/C6</f>
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>